<commit_message>
Change "Other Exts" to \Other"
</commit_message>
<xml_diff>
--- a/Contacts - REDACTED.xlsx
+++ b/Contacts - REDACTED.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="1" r:id="rId1"/>
     <sheet name="Support" sheetId="2" r:id="rId2"/>
-    <sheet name="Other Exts" sheetId="3" r:id="rId3"/>
+    <sheet name="Other" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Personnel[]</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="183">
   <si>
     <t>Last</t>
   </si>
@@ -441,55 +441,97 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Ext</t>
-  </si>
-  <si>
     <t>6N</t>
   </si>
   <si>
+    <t>Ext: 5062</t>
+  </si>
+  <si>
     <t>BioMed</t>
   </si>
   <si>
+    <t>Ext: 2088</t>
+  </si>
+  <si>
     <t>2067 is listed in the Phone Directory, but this forwards to the operator.</t>
   </si>
   <si>
     <t>Cancer Center</t>
   </si>
   <si>
+    <t>Ext: 2497</t>
+  </si>
+  <si>
     <t>CRMC Cafeteria Menu</t>
   </si>
   <si>
+    <t>Ext: 2469</t>
+  </si>
+  <si>
     <t>E1</t>
   </si>
   <si>
+    <t>Ext: 2225</t>
+  </si>
+  <si>
     <t>E2</t>
   </si>
   <si>
+    <t>Ext: 2615</t>
+  </si>
+  <si>
     <t>EVS</t>
   </si>
   <si>
+    <t>Ext: 2672</t>
+  </si>
+  <si>
     <t>Nuc Med</t>
   </si>
   <si>
+    <t>Ext: 3135</t>
+  </si>
+  <si>
     <t>Oncology fax</t>
   </si>
   <si>
+    <t>Ext: 5666</t>
+  </si>
+  <si>
     <t>Phone beside D4 computer</t>
   </si>
   <si>
+    <t>Ext: 2224</t>
+  </si>
+  <si>
     <t>Plant Facilities (maintenance)</t>
   </si>
   <si>
+    <t>Ext: 2588</t>
+  </si>
+  <si>
     <t>Non-medical (contact BioMed for medical)</t>
   </si>
   <si>
     <t>Sim</t>
   </si>
   <si>
+    <t>Ext: 2203</t>
+  </si>
+  <si>
+    <t>Ext: 2270</t>
+  </si>
+  <si>
     <t>Transfer Center</t>
   </si>
   <si>
+    <t>Ext: 2017</t>
+  </si>
+  <si>
     <t>Voicemail</t>
+  </si>
+  <si>
+    <t>Ext: 5000</t>
   </si>
   <si>
     <t>[redacted]</t>
@@ -746,14 +788,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="OtherExts" displayName="OtherExts" ref="A1:C16" totalsRowShown="0">
-  <autoFilter ref="A1:C16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="OtherExts" displayName="OtherExts" ref="A1:C17" totalsRowShown="0">
+  <autoFilter ref="A1:C17"/>
   <sortState ref="A2:C16">
     <sortCondition ref="A1:A16"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Description"/>
-    <tableColumn id="3" name="Ext" dataDxfId="1"/>
+    <tableColumn id="3" name="Ph" dataDxfId="1"/>
     <tableColumn id="2" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1028,8 +1070,8 @@
   </sheetPr>
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1068,10 +1110,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1080,18 +1122,18 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -1100,7 +1142,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>11</v>
@@ -1108,10 +1150,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -1120,7 +1162,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>13</v>
@@ -1131,10 +1173,10 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -1143,18 +1185,18 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1163,7 +1205,7 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>18</v>
@@ -1171,10 +1213,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1183,7 +1225,7 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>20</v>
@@ -1191,10 +1233,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -1203,7 +1245,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>23</v>
@@ -1211,10 +1253,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -1223,18 +1265,18 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1243,7 +1285,7 @@
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>27</v>
@@ -1251,10 +1293,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1263,7 +1305,7 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>29</v>
@@ -1271,10 +1313,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -1283,18 +1325,18 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -1303,18 +1345,18 @@
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
@@ -1324,15 +1366,15 @@
       </c>
       <c r="E14"/>
       <c r="F14" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C15" t="s">
         <v>32</v>
@@ -1341,18 +1383,18 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -1362,15 +1404,15 @@
       </c>
       <c r="E16"/>
       <c r="F16" s="2" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
@@ -1380,22 +1422,22 @@
       </c>
       <c r="E17"/>
       <c r="F17" s="2" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
       </c>
       <c r="E18"/>
       <c r="F18" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>35</v>
@@ -1403,10 +1445,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
         <v>36</v>
@@ -1415,10 +1457,10 @@
         <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>38</v>
@@ -1426,10 +1468,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1438,7 +1480,7 @@
         <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>40</v>
@@ -1449,10 +1491,10 @@
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -1461,18 +1503,18 @@
         <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
@@ -1481,27 +1523,27 @@
         <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>45</v>
@@ -1509,10 +1551,10 @@
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C24" t="s">
         <v>46</v>
@@ -1521,10 +1563,10 @@
         <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>35</v>
@@ -1532,10 +1574,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
@@ -1544,18 +1586,18 @@
         <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -1564,7 +1606,7 @@
         <v>48</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>49</v>
@@ -1572,10 +1614,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C27" t="s">
         <v>36</v>
@@ -1584,10 +1626,10 @@
         <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>38</v>
@@ -1595,10 +1637,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -1607,7 +1649,7 @@
         <v>50</v>
       </c>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>51</v>
@@ -1618,10 +1660,10 @@
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -1630,18 +1672,18 @@
         <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
         <v>54</v>
@@ -1650,10 +1692,10 @@
         <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>56</v>
@@ -1661,10 +1703,10 @@
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -1673,18 +1715,18 @@
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C32" t="s">
         <v>21</v>
@@ -1693,7 +1735,7 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>35</v>
@@ -1701,10 +1743,10 @@
     </row>
     <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C33" t="s">
         <v>46</v>
@@ -1713,10 +1755,10 @@
         <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>35</v>
@@ -1724,10 +1766,10 @@
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
         <v>46</v>
@@ -1736,10 +1778,10 @@
         <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>35</v>
@@ -1747,10 +1789,10 @@
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B35" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
@@ -1759,10 +1801,10 @@
         <v>37</v>
       </c>
       <c r="E35" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>38</v>
@@ -1770,10 +1812,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -1782,10 +1824,10 @@
         <v>58</v>
       </c>
       <c r="E36" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>59</v>
@@ -1793,10 +1835,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
@@ -1805,18 +1847,18 @@
         <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C38" t="s">
         <v>32</v>
@@ -1825,7 +1867,7 @@
         <v>60</v>
       </c>
       <c r="E38" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>61</v>
@@ -1833,10 +1875,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C39" t="s">
         <v>62</v>
@@ -1846,30 +1888,30 @@
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C40" t="s">
         <v>64</v>
       </c>
       <c r="E40"/>
       <c r="F40" s="2" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
         <v>65</v>
@@ -1878,7 +1920,7 @@
         <v>22</v>
       </c>
       <c r="E41" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>66</v>
@@ -1886,10 +1928,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -1898,7 +1940,7 @@
         <v>67</v>
       </c>
       <c r="E42" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>68</v>
@@ -1906,10 +1948,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C43" t="s">
         <v>62</v>
@@ -1918,15 +1960,15 @@
         <v>69</v>
       </c>
       <c r="E43" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B44" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -1935,18 +1977,18 @@
         <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B45" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
@@ -1955,7 +1997,7 @@
         <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>72</v>
@@ -1966,10 +2008,10 @@
     </row>
     <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B46" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -1978,18 +2020,18 @@
         <v>74</v>
       </c>
       <c r="E46" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B47" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
@@ -1998,7 +2040,7 @@
         <v>75</v>
       </c>
       <c r="E47" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>76</v>
@@ -2009,10 +2051,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B48" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C48" t="s">
         <v>62</v>
@@ -2021,7 +2063,7 @@
         <v>78</v>
       </c>
       <c r="E48" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>79</v>
@@ -2029,10 +2071,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B49" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C49" t="s">
         <v>62</v>
@@ -2041,18 +2083,18 @@
         <v>80</v>
       </c>
       <c r="E49" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C50" t="s">
         <v>32</v>
@@ -2061,10 +2103,10 @@
         <v>81</v>
       </c>
       <c r="E50" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>82</v>
@@ -2072,10 +2114,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
@@ -2084,7 +2126,7 @@
         <v>19</v>
       </c>
       <c r="E51" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>83</v>
@@ -2092,10 +2134,10 @@
     </row>
     <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s">
         <v>46</v>
@@ -2104,10 +2146,10 @@
         <v>47</v>
       </c>
       <c r="E52" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>35</v>
@@ -2115,10 +2157,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
@@ -2127,7 +2169,7 @@
         <v>84</v>
       </c>
       <c r="E53" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>85</v>
@@ -2138,10 +2180,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B54" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C54" t="s">
         <v>62</v>
@@ -2150,7 +2192,7 @@
         <v>87</v>
       </c>
       <c r="E54" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>88</v>
@@ -2158,10 +2200,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B55" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C55" t="s">
         <v>9</v>
@@ -2170,7 +2212,7 @@
         <v>89</v>
       </c>
       <c r="E55" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>90</v>
@@ -2181,10 +2223,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B56" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
@@ -2193,7 +2235,7 @@
         <v>53</v>
       </c>
       <c r="E56" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>92</v>
@@ -2201,10 +2243,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C57" t="s">
         <v>93</v>
@@ -2213,18 +2255,18 @@
         <v>94</v>
       </c>
       <c r="E57" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B58" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C58" t="s">
         <v>95</v>
@@ -2233,7 +2275,7 @@
         <v>96</v>
       </c>
       <c r="E58" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>35</v>
@@ -2241,10 +2283,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C59" t="s">
         <v>97</v>
@@ -2256,10 +2298,10 @@
     </row>
     <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B60" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -2268,18 +2310,18 @@
         <v>22</v>
       </c>
       <c r="E60" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B61" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C61" t="s">
         <v>36</v>
@@ -2288,10 +2330,10 @@
         <v>37</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>38</v>
@@ -2299,10 +2341,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B62" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C62" t="s">
         <v>99</v>
@@ -2311,10 +2353,10 @@
         <v>100</v>
       </c>
       <c r="E62" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>101</v>
@@ -2322,10 +2364,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B63" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C63" t="s">
         <v>99</v>
@@ -2337,10 +2379,10 @@
     </row>
     <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B64" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -2349,18 +2391,18 @@
         <v>102</v>
       </c>
       <c r="E64" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B65" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C65" t="s">
         <v>36</v>
@@ -2369,18 +2411,18 @@
         <v>103</v>
       </c>
       <c r="E65" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B66" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C66" t="s">
         <v>54</v>
@@ -2389,7 +2431,7 @@
         <v>104</v>
       </c>
       <c r="E66" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>105</v>
@@ -2397,10 +2439,10 @@
     </row>
     <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C67" t="s">
         <v>36</v>
@@ -2409,10 +2451,10 @@
         <v>37</v>
       </c>
       <c r="E67" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>38</v>
@@ -2420,14 +2462,14 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C68" t="s">
         <v>106</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2444,8 +2486,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2482,10 +2524,10 @@
         <v>108</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>109</v>
@@ -2499,13 +2541,13 @@
         <v>111</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>112</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
@@ -2516,10 +2558,10 @@
         <v>114</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>115</v>
@@ -2533,13 +2575,13 @@
         <v>116</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>117</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2550,10 +2592,10 @@
         <v>119</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>120</v>
@@ -2567,10 +2609,10 @@
         <v>121</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>122</v>
@@ -2584,7 +2626,7 @@
         <v>123</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>124</v>
@@ -2601,10 +2643,10 @@
         <v>127</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>128</v>
@@ -2618,13 +2660,13 @@
         <v>129</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>130</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.2">
@@ -2635,10 +2677,10 @@
         <v>132</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>133</v>
@@ -2664,16 +2706,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2682,7 +2724,7 @@
         <v>134</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>135</v>
+        <v>5</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>6</v>
@@ -2690,10 +2732,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="B2" s="12">
-        <v>5062</v>
       </c>
       <c r="C2" s="12"/>
     </row>
@@ -2701,102 +2743,102 @@
       <c r="A3" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="12">
-        <v>2088</v>
+      <c r="B3" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="12">
-        <v>2497</v>
+        <v>140</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>141</v>
       </c>
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" s="12">
-        <v>2469</v>
+        <v>142</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>143</v>
       </c>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B6" s="12">
-        <v>2225</v>
+        <v>144</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>145</v>
       </c>
       <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" s="12">
-        <v>2615</v>
+        <v>146</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B8" s="12">
-        <v>2672</v>
+        <v>148</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" s="12">
-        <v>3135</v>
+        <v>150</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10" s="12">
-        <v>5666</v>
+        <v>152</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" s="12">
-        <v>2224</v>
+        <v>154</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>155</v>
       </c>
       <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="12">
-        <v>2588</v>
+        <v>156</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>149</v>
-      </c>
-      <c r="B13" s="12">
-        <v>2203</v>
+        <v>159</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="C13" s="12"/>
     </row>
@@ -2804,28 +2846,37 @@
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="12">
-        <v>2270</v>
+      <c r="B14" s="12" t="s">
+        <v>161</v>
       </c>
       <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="12">
-        <v>2017</v>
+        <v>162</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B16" s="12">
-        <v>5000</v>
+        <v>164</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>165</v>
       </c>
       <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Redact emails and phone numbers instead of whole value for certain columns
</commit_message>
<xml_diff>
--- a/Contacts - REDACTED.xlsx
+++ b/Contacts - REDACTED.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="189">
   <si>
     <t>Last</t>
   </si>
@@ -368,6 +368,9 @@
     <t>786-288-0369</t>
   </si>
   <si>
+    <t>service-usa@iba-group.com</t>
+  </si>
+  <si>
     <t>helpcenter.iba-dosimetry.com</t>
   </si>
   <si>
@@ -377,13 +380,15 @@
     <t>800-323-8830</t>
   </si>
   <si>
-    <t>ext 3, 1 for myLDR
-Account #163258</t>
+    <t>myldr@landauer.com</t>
   </si>
   <si>
     <t>866-421-2536</t>
   </si>
   <si>
+    <t>support@mimsoftware.com</t>
+  </si>
+  <si>
     <t>mimsoftware.com/support?product=MIM.6.9.3.J510-01</t>
   </si>
   <si>
@@ -399,6 +404,9 @@
     <t>877-778-3849</t>
   </si>
   <si>
+    <t>support@raysearchlabs.com</t>
+  </si>
+  <si>
     <t>ext 1 for customer service</t>
   </si>
   <si>
@@ -406,9 +414,6 @@
   </si>
   <si>
     <t>rjyoung.com</t>
-  </si>
-  <si>
-    <t>Equipment ID: AAA58116</t>
   </si>
   <si>
     <t>Scandidos</t>
@@ -418,6 +423,9 @@
 Global: +46 18-472-30-30</t>
   </si>
   <si>
+    <t>support@scandidos.com</t>
+  </si>
+  <si>
     <t>Call global if no one answers U.S.
 File sharing: sprend.com</t>
   </si>
@@ -425,6 +433,9 @@
     <t>1-866-368-4807</t>
   </si>
   <si>
+    <t>support@tomotherapy.com</t>
+  </si>
+  <si>
     <t>www.accuray.com/service-requests/</t>
   </si>
   <si>
@@ -432,6 +443,9 @@
   </si>
   <si>
     <t>1-888-827-4265</t>
+  </si>
+  <si>
+    <t>support@varian.com</t>
   </si>
   <si>
     <t>ext 2 for Clinical
@@ -481,9 +495,6 @@
   </si>
   <si>
     <t>EVS</t>
-  </si>
-  <si>
-    <t>Ext: 2672</t>
   </si>
   <si>
     <t>Nuc Med</t>
@@ -596,7 +607,15 @@
 Ext: 2188</t>
   </si>
   <si>
-    <t/>
+    <t>Ext: 2672
+Fax: [redacted]</t>
+  </si>
+  <si>
+    <t>Equipment ID: [redacted]</t>
+  </si>
+  <si>
+    <t>ext 3, 1 for myLDR
+Account #[redacted]</t>
   </si>
 </sst>
 </file>
@@ -647,7 +666,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -684,6 +703,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -755,7 +777,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Personnel" displayName="Personnel" ref="A1:G68" totalsRowShown="0">
   <autoFilter ref="A1:G68"/>
   <sortState ref="A2:G68">
-    <sortCondition ref="A1:A68"/>
+    <sortCondition ref="A2:A68"/>
+    <sortCondition ref="B2:B68"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="Last"/>
@@ -788,10 +811,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="OtherExts" displayName="OtherExts" ref="A1:C17" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Other" displayName="Other" ref="A1:C17" totalsRowShown="0">
   <autoFilter ref="A1:C17"/>
-  <sortState ref="A2:C16">
-    <sortCondition ref="A1:A16"/>
+  <sortState ref="A2:C17">
+    <sortCondition ref="A1:A17"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Description"/>
@@ -1070,8 +1093,8 @@
   </sheetPr>
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1110,10 +1133,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1122,18 +1145,18 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -1142,7 +1165,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>11</v>
@@ -1150,10 +1173,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -1162,7 +1185,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>13</v>
@@ -1173,10 +1196,10 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -1185,18 +1208,18 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1205,7 +1228,7 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>18</v>
@@ -1213,10 +1236,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1225,7 +1248,7 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>20</v>
@@ -1233,10 +1256,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -1245,7 +1268,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>23</v>
@@ -1253,10 +1276,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -1265,18 +1288,18 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1285,7 +1308,7 @@
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>27</v>
@@ -1293,10 +1316,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1305,7 +1328,7 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>29</v>
@@ -1313,10 +1336,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -1325,18 +1348,18 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -1345,18 +1368,18 @@
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
@@ -1366,15 +1389,15 @@
       </c>
       <c r="E14"/>
       <c r="F14" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C15" t="s">
         <v>32</v>
@@ -1383,18 +1406,18 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -1404,15 +1427,15 @@
       </c>
       <c r="E16"/>
       <c r="F16" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
@@ -1422,22 +1445,22 @@
       </c>
       <c r="E17"/>
       <c r="F17" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B18" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
       </c>
       <c r="E18"/>
       <c r="F18" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>35</v>
@@ -1445,10 +1468,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C19" t="s">
         <v>36</v>
@@ -1457,10 +1480,10 @@
         <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>38</v>
@@ -1468,10 +1491,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1480,7 +1503,7 @@
         <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>40</v>
@@ -1491,10 +1514,10 @@
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -1503,18 +1526,18 @@
         <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
@@ -1523,27 +1546,27 @@
         <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>45</v>
@@ -1551,10 +1574,10 @@
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B24" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C24" t="s">
         <v>46</v>
@@ -1563,10 +1586,10 @@
         <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>35</v>
@@ -1574,10 +1597,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
@@ -1586,18 +1609,18 @@
         <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B26" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -1606,7 +1629,7 @@
         <v>48</v>
       </c>
       <c r="E26" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>49</v>
@@ -1614,10 +1637,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C27" t="s">
         <v>36</v>
@@ -1626,10 +1649,10 @@
         <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>38</v>
@@ -1637,10 +1660,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -1649,7 +1672,7 @@
         <v>50</v>
       </c>
       <c r="E28" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>51</v>
@@ -1660,10 +1683,10 @@
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B29" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -1672,18 +1695,18 @@
         <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C30" t="s">
         <v>54</v>
@@ -1692,10 +1715,10 @@
         <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>56</v>
@@ -1703,10 +1726,10 @@
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -1715,18 +1738,18 @@
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B32" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C32" t="s">
         <v>21</v>
@@ -1735,7 +1758,7 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>35</v>
@@ -1743,10 +1766,10 @@
     </row>
     <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B33" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C33" t="s">
         <v>46</v>
@@ -1755,10 +1778,10 @@
         <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>35</v>
@@ -1766,10 +1789,10 @@
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C34" t="s">
         <v>46</v>
@@ -1778,10 +1801,10 @@
         <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>35</v>
@@ -1789,10 +1812,10 @@
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
@@ -1801,10 +1824,10 @@
         <v>37</v>
       </c>
       <c r="E35" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>38</v>
@@ -1812,10 +1835,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B36" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -1824,10 +1847,10 @@
         <v>58</v>
       </c>
       <c r="E36" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>59</v>
@@ -1835,10 +1858,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B37" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
@@ -1847,18 +1870,18 @@
         <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C38" t="s">
         <v>32</v>
@@ -1867,7 +1890,7 @@
         <v>60</v>
       </c>
       <c r="E38" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>61</v>
@@ -1875,10 +1898,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B39" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C39" t="s">
         <v>62</v>
@@ -1888,30 +1911,30 @@
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B40" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
         <v>64</v>
       </c>
       <c r="E40"/>
       <c r="F40" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C41" t="s">
         <v>65</v>
@@ -1920,7 +1943,7 @@
         <v>22</v>
       </c>
       <c r="E41" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>66</v>
@@ -1928,10 +1951,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -1940,7 +1963,7 @@
         <v>67</v>
       </c>
       <c r="E42" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>68</v>
@@ -1948,10 +1971,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C43" t="s">
         <v>62</v>
@@ -1960,15 +1983,15 @@
         <v>69</v>
       </c>
       <c r="E43" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B44" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -1977,18 +2000,18 @@
         <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B45" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
@@ -1997,7 +2020,7 @@
         <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>72</v>
@@ -2008,10 +2031,10 @@
     </row>
     <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B46" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -2020,18 +2043,18 @@
         <v>74</v>
       </c>
       <c r="E46" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
@@ -2040,7 +2063,7 @@
         <v>75</v>
       </c>
       <c r="E47" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>76</v>
@@ -2051,10 +2074,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B48" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C48" t="s">
         <v>62</v>
@@ -2063,7 +2086,7 @@
         <v>78</v>
       </c>
       <c r="E48" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>79</v>
@@ -2071,10 +2094,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B49" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C49" t="s">
         <v>62</v>
@@ -2083,18 +2106,18 @@
         <v>80</v>
       </c>
       <c r="E49" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B50" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C50" t="s">
         <v>32</v>
@@ -2103,10 +2126,10 @@
         <v>81</v>
       </c>
       <c r="E50" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>82</v>
@@ -2114,10 +2137,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B51" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
@@ -2126,7 +2149,7 @@
         <v>19</v>
       </c>
       <c r="E51" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>83</v>
@@ -2134,10 +2157,10 @@
     </row>
     <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B52" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C52" t="s">
         <v>46</v>
@@ -2146,10 +2169,10 @@
         <v>47</v>
       </c>
       <c r="E52" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>35</v>
@@ -2157,10 +2180,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B53" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
@@ -2169,7 +2192,7 @@
         <v>84</v>
       </c>
       <c r="E53" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>85</v>
@@ -2180,10 +2203,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C54" t="s">
         <v>62</v>
@@ -2192,7 +2215,7 @@
         <v>87</v>
       </c>
       <c r="E54" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>88</v>
@@ -2200,10 +2223,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C55" t="s">
         <v>9</v>
@@ -2212,7 +2235,7 @@
         <v>89</v>
       </c>
       <c r="E55" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>90</v>
@@ -2223,10 +2246,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B56" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
@@ -2235,7 +2258,7 @@
         <v>53</v>
       </c>
       <c r="E56" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>92</v>
@@ -2243,10 +2266,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B57" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C57" t="s">
         <v>93</v>
@@ -2255,18 +2278,18 @@
         <v>94</v>
       </c>
       <c r="E57" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B58" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C58" t="s">
         <v>95</v>
@@ -2275,7 +2298,7 @@
         <v>96</v>
       </c>
       <c r="E58" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>35</v>
@@ -2283,10 +2306,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B59" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C59" t="s">
         <v>97</v>
@@ -2298,10 +2321,10 @@
     </row>
     <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B60" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -2310,18 +2333,18 @@
         <v>22</v>
       </c>
       <c r="E60" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B61" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C61" t="s">
         <v>36</v>
@@ -2330,10 +2353,10 @@
         <v>37</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>38</v>
@@ -2341,10 +2364,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C62" t="s">
         <v>99</v>
@@ -2353,10 +2376,10 @@
         <v>100</v>
       </c>
       <c r="E62" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>101</v>
@@ -2364,10 +2387,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B63" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C63" t="s">
         <v>99</v>
@@ -2379,10 +2402,10 @@
     </row>
     <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B64" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -2391,18 +2414,18 @@
         <v>102</v>
       </c>
       <c r="E64" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B65" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C65" t="s">
         <v>36</v>
@@ -2411,18 +2434,18 @@
         <v>103</v>
       </c>
       <c r="E65" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B66" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C66" t="s">
         <v>54</v>
@@ -2431,7 +2454,7 @@
         <v>104</v>
       </c>
       <c r="E66" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>105</v>
@@ -2439,10 +2462,10 @@
     </row>
     <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B67" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C67" t="s">
         <v>36</v>
@@ -2451,10 +2474,10 @@
         <v>37</v>
       </c>
       <c r="E67" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>38</v>
@@ -2462,14 +2485,14 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C68" t="s">
         <v>106</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2487,7 +2510,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2523,12 +2546,8 @@
       <c r="B2" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>182</v>
-      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
         <v>109</v>
       </c>
@@ -2541,30 +2560,26 @@
         <v>111</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>166</v>
+        <v>112</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>182</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>182</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D4" s="6"/>
       <c r="E4" s="10" t="s">
-        <v>115</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2572,33 +2587,27 @@
         <v>54</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>182</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>182</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2606,16 +2615,14 @@
         <v>62</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>182</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="10" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2623,33 +2630,29 @@
         <v>106</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>182</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C8" s="9"/>
       <c r="D8" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>182</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D9" s="6"/>
       <c r="E9" s="10" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2657,44 +2660,40 @@
         <v>24</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>182</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>182</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="D11" s="6"/>
       <c r="E11" s="10" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="support@varian.com"/>
-    <hyperlink ref="C7" r:id="rId2" display="support@raysearchlabs.com"/>
-    <hyperlink ref="C10" r:id="rId3" display="support@tomotherapy.com"/>
+    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C10" r:id="rId3"/>
     <hyperlink ref="D10" r:id="rId4"/>
-    <hyperlink ref="C4" r:id="rId5" display="myldr@landauer.com"/>
-    <hyperlink ref="C9" r:id="rId6" display="support@scandidos.com"/>
-    <hyperlink ref="C3" r:id="rId7" display="service-usa@iba-group.com"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="C3" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2709,19 +2708,19 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="12" customWidth="1"/>
     <col min="3" max="3" width="55.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>5</v>
@@ -2732,156 +2731,157 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>149</v>
+        <v>153</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>158</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C13" s="12"/>
+        <v>161</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>24</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>168</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C17" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>